<commit_message>
Added formulas to excel sheet
need to add inventory items and costs/price points to the sheet, and
change formulas to fit.
</commit_message>
<xml_diff>
--- a/MakoInventoryControl.xlsx
+++ b/MakoInventoryControl.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,13 +11,42 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Item:</t>
+  </si>
+  <si>
+    <t>Number on Hand:</t>
+  </si>
+  <si>
+    <t>Our Cost per Item</t>
+  </si>
+  <si>
+    <t>Total Value of Item on Hand</t>
+  </si>
+  <si>
+    <t>Customers Cost per item</t>
+  </si>
+  <si>
+    <t>Total Value of Customer Cost</t>
+  </si>
+  <si>
+    <t>Profit per Item</t>
+  </si>
+  <si>
+    <t>Profit of Item on Hand</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +54,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,18 +84,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +408,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1">
+        <f>PRODUCT(B2, C2)</f>
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <f>PRODUCT(B2,E2)</f>
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <f>SUM(E2,-C2)</f>
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <f>PRODUCT(G2,B2)</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>PRODUCT(B3,C3)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>PRODUCT(B3,E3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>SUM(E3,-C3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>PRODUCT(G3,B3)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Resume data entry from pg 325 in connor book
</commit_message>
<xml_diff>
--- a/MakoInventoryControl.xlsx
+++ b/MakoInventoryControl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Item:</t>
   </si>
@@ -87,28 +87,313 @@
     <t>4" PVC repair coupling</t>
   </si>
   <si>
-    <t>1.5" female adapt</t>
-  </si>
-  <si>
-    <t>2" female adapt</t>
-  </si>
-  <si>
-    <t>3" female adapt</t>
-  </si>
-  <si>
-    <t>4" female adapt</t>
-  </si>
-  <si>
-    <t>1.5" male adapt</t>
-  </si>
-  <si>
-    <t>2" male adapt</t>
-  </si>
-  <si>
-    <t>3" male adapt</t>
-  </si>
-  <si>
-    <t>4" male adapt</t>
+    <t>1.5" female adapt PVC</t>
+  </si>
+  <si>
+    <t>2" female adapt PVC</t>
+  </si>
+  <si>
+    <t>3" female adapt PVC</t>
+  </si>
+  <si>
+    <t>4" female adapt PVC</t>
+  </si>
+  <si>
+    <t>1.5" male adapt PVC</t>
+  </si>
+  <si>
+    <t>2" male adapt PVC</t>
+  </si>
+  <si>
+    <t>3" male adapt PVC</t>
+  </si>
+  <si>
+    <t>4" male adapt PVC</t>
+  </si>
+  <si>
+    <t>1.5" Female Trap Adapt with washers/nut PVC</t>
+  </si>
+  <si>
+    <t>1.5"x1.25" Female Trap Adapt with washers/nut PVC</t>
+  </si>
+  <si>
+    <t>1.5"x1.25" Female Trap Adapt with washers/nut both 1.5" washer and 1.25" washer PVC</t>
+  </si>
+  <si>
+    <t>1.5"x1.25" male trap adapt with nut and washer PVC</t>
+  </si>
+  <si>
+    <t>1.5" male trap adapt with nut and washer PVC</t>
+  </si>
+  <si>
+    <t>2" male trap adapt  PVC</t>
+  </si>
+  <si>
+    <t>1.5" male cleanout with plug PVC</t>
+  </si>
+  <si>
+    <t>2" male cleanout with plug PVC</t>
+  </si>
+  <si>
+    <t>3" male cleanout with plug PVC</t>
+  </si>
+  <si>
+    <t>4" male cleanout with plug PVC</t>
+  </si>
+  <si>
+    <t>1.5" male cleanout w/o plug PVC</t>
+  </si>
+  <si>
+    <t>2" male cleanout w/o plug PVC</t>
+  </si>
+  <si>
+    <t>3" male cleanout w/o plug PVC</t>
+  </si>
+  <si>
+    <t>4" male cleanout w/o plug PVC</t>
+  </si>
+  <si>
+    <t>1.5" cleanout plug PVC</t>
+  </si>
+  <si>
+    <t>2" cleanout plug PVC</t>
+  </si>
+  <si>
+    <t>3" cleanout plug PVC</t>
+  </si>
+  <si>
+    <t>4" cleanout plug PVC</t>
+  </si>
+  <si>
+    <t>1.5" cap PVC</t>
+  </si>
+  <si>
+    <t>2" cap PVC</t>
+  </si>
+  <si>
+    <t>3" cap PVC</t>
+  </si>
+  <si>
+    <t>4" cap PVC</t>
+  </si>
+  <si>
+    <t>1.5"x1.25" PVC Flush Bushing</t>
+  </si>
+  <si>
+    <t>2"x1.5" PVC Flush Bushing</t>
+  </si>
+  <si>
+    <t>3"x1.5" PVC Flush Bushing</t>
+  </si>
+  <si>
+    <t>3"x2" PVC Flush Bushing</t>
+  </si>
+  <si>
+    <t>4"x2" PVC Flush Bushing</t>
+  </si>
+  <si>
+    <t>4"x3" PVC Flush Bushing</t>
+  </si>
+  <si>
+    <t>1.5" No Hub Adapter</t>
+  </si>
+  <si>
+    <t>2" No Hub Adapter</t>
+  </si>
+  <si>
+    <t>3" No Hub Adapter</t>
+  </si>
+  <si>
+    <t>4" No Hub Adapter</t>
+  </si>
+  <si>
+    <t>4"x3" No Hub Adapter</t>
+  </si>
+  <si>
+    <t>1.5" PVC 90</t>
+  </si>
+  <si>
+    <t>2" PVC 90</t>
+  </si>
+  <si>
+    <t>3" PVC 90</t>
+  </si>
+  <si>
+    <t>4" PVC 90</t>
+  </si>
+  <si>
+    <t>3"x3"x1.5" PVC 90 with side out</t>
+  </si>
+  <si>
+    <t>3"x3"x2" PVC 90 with side out</t>
+  </si>
+  <si>
+    <t>3"x3"x1.5" PVC 90 heel out</t>
+  </si>
+  <si>
+    <t>3"x3"x2" PVC 90 heel out</t>
+  </si>
+  <si>
+    <t>4"x4"x2" PVC 90 heel out</t>
+  </si>
+  <si>
+    <t>1.5" PVC Street 90</t>
+  </si>
+  <si>
+    <t>2" PVC Street 90</t>
+  </si>
+  <si>
+    <t>3" PVC Street 90</t>
+  </si>
+  <si>
+    <t>4" PVC Street 90</t>
+  </si>
+  <si>
+    <t>1.5" PVC LongTurn 90</t>
+  </si>
+  <si>
+    <t>2" PVC LongTurn 90</t>
+  </si>
+  <si>
+    <t>3" PVC LongTurn 90</t>
+  </si>
+  <si>
+    <t>4" PVC LongTurn 90</t>
+  </si>
+  <si>
+    <t>1.5" PVC LongTurn Street 90</t>
+  </si>
+  <si>
+    <t>2" PVC LongTurn Street 90</t>
+  </si>
+  <si>
+    <t>3" PVC LongTurn Street 90</t>
+  </si>
+  <si>
+    <t>4" PVC LongTurn Street 90</t>
+  </si>
+  <si>
+    <t>1.5" PVC 60</t>
+  </si>
+  <si>
+    <t>2" PVC 60</t>
+  </si>
+  <si>
+    <t>3" PVC 60</t>
+  </si>
+  <si>
+    <t>4" PVC 60</t>
+  </si>
+  <si>
+    <t>1.5" PVC street 60</t>
+  </si>
+  <si>
+    <t>2" PVC street 60</t>
+  </si>
+  <si>
+    <t>3" PVC street 60</t>
+  </si>
+  <si>
+    <t>4" PVC street 60</t>
+  </si>
+  <si>
+    <t>1.5" PVC 45</t>
+  </si>
+  <si>
+    <t>2" PVC 45</t>
+  </si>
+  <si>
+    <t>3" PVC 45</t>
+  </si>
+  <si>
+    <t>4" PVC 45</t>
+  </si>
+  <si>
+    <t>1.5" PVC street 45</t>
+  </si>
+  <si>
+    <t>2" PVC street 45</t>
+  </si>
+  <si>
+    <t>3" PVC street 45</t>
+  </si>
+  <si>
+    <t>4" PVC street 45</t>
+  </si>
+  <si>
+    <t>1.5" PVC 22</t>
+  </si>
+  <si>
+    <t>2" PVC 22</t>
+  </si>
+  <si>
+    <t>3" PVC 22</t>
+  </si>
+  <si>
+    <t>4" PVC 22</t>
+  </si>
+  <si>
+    <t>1.5" PVC Street 22</t>
+  </si>
+  <si>
+    <t>2" PVC Street 22</t>
+  </si>
+  <si>
+    <t>3" PVC Street 22</t>
+  </si>
+  <si>
+    <t>4" PVC Street 22</t>
+  </si>
+  <si>
+    <t>1.5" PVC twin 90</t>
+  </si>
+  <si>
+    <t>2" PVC twin 90</t>
+  </si>
+  <si>
+    <t>3" PVC twin 90</t>
+  </si>
+  <si>
+    <t>2"X1.5"X1.5" PVC twin 90</t>
+  </si>
+  <si>
+    <t>3"x4" Reducing Closet Bend (HxH)</t>
+  </si>
+  <si>
+    <t>3"x4" Reducing Closet Bend (HxSpg)</t>
+  </si>
+  <si>
+    <t>1.5" PVC T</t>
+  </si>
+  <si>
+    <t>2" PVC T</t>
+  </si>
+  <si>
+    <t>3" PVC T</t>
+  </si>
+  <si>
+    <t>4" PVC T</t>
+  </si>
+  <si>
+    <t>2"x1.5" PVC T</t>
+  </si>
+  <si>
+    <t>3"x1.5" PVC T</t>
+  </si>
+  <si>
+    <t>3"x2" PVC T</t>
+  </si>
+  <si>
+    <t>4"x1.5" PVC T</t>
+  </si>
+  <si>
+    <t>4"x2" PVC T</t>
+  </si>
+  <si>
+    <t>4"x3" PVC T</t>
+  </si>
+  <si>
+    <t>Resume on Page 325 in connors book</t>
   </si>
 </sst>
 </file>
@@ -478,14 +763,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
@@ -747,6 +1033,763 @@
       </c>
       <c r="C24">
         <v>10.85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>7.69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>3.41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33">
+        <v>8.2200000000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34">
+        <v>13.09</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38">
+        <v>9.57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43">
+        <v>2.71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45">
+        <v>7.55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46">
+        <v>10.78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51">
+        <v>9.74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52">
+        <v>4.97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53">
+        <v>8.74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55">
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56">
+        <v>6.59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57">
+        <v>11.32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61">
+        <v>12.91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63">
+        <v>12.94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64">
+        <v>13.25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65">
+        <v>11.41</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66">
+        <v>22.52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69">
+        <v>7.02</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70">
+        <v>13.21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>77</v>
+      </c>
+      <c r="C71">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73">
+        <v>8.35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>80</v>
+      </c>
+      <c r="C74">
+        <v>15.94</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75">
+        <v>5.0199999999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C77">
+        <v>15.14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>84</v>
+      </c>
+      <c r="C78">
+        <v>23.32</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>86</v>
+      </c>
+      <c r="C80">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>87</v>
+      </c>
+      <c r="C81">
+        <v>12.17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82">
+        <v>18.84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>89</v>
+      </c>
+      <c r="C83">
+        <v>5.97</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>90</v>
+      </c>
+      <c r="C84">
+        <v>7.78</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>91</v>
+      </c>
+      <c r="C85">
+        <v>16.77</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86">
+        <v>25.2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>93</v>
+      </c>
+      <c r="C87">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>94</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>95</v>
+      </c>
+      <c r="C89">
+        <v>5.87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>96</v>
+      </c>
+      <c r="C90">
+        <v>10.29</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>97</v>
+      </c>
+      <c r="C91">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>98</v>
+      </c>
+      <c r="C92">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>99</v>
+      </c>
+      <c r="C93">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94">
+        <v>9.51</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>101</v>
+      </c>
+      <c r="C95">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>102</v>
+      </c>
+      <c r="C96">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>103</v>
+      </c>
+      <c r="C97">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>104</v>
+      </c>
+      <c r="C98">
+        <v>9.1300000000000008</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>105</v>
+      </c>
+      <c r="C99">
+        <v>5.32</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>106</v>
+      </c>
+      <c r="C100">
+        <v>5.69</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>107</v>
+      </c>
+      <c r="C101">
+        <v>8.94</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>108</v>
+      </c>
+      <c r="C102">
+        <v>13.05</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>109</v>
+      </c>
+      <c r="C103">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>110</v>
+      </c>
+      <c r="C104">
+        <v>7.59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>111</v>
+      </c>
+      <c r="C105">
+        <v>20.05</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>112</v>
+      </c>
+      <c r="C106">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>113</v>
+      </c>
+      <c r="C107">
+        <v>10.51</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>114</v>
+      </c>
+      <c r="C108">
+        <v>20.04</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>115</v>
+      </c>
+      <c r="C109">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>116</v>
+      </c>
+      <c r="C110">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>117</v>
+      </c>
+      <c r="C111">
+        <v>9.5399999999999991</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>118</v>
+      </c>
+      <c r="C112">
+        <v>17.53</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>119</v>
+      </c>
+      <c r="C113">
+        <v>3.21</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>120</v>
+      </c>
+      <c r="C114">
+        <v>6.97</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>121</v>
+      </c>
+      <c r="C115">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>122</v>
+      </c>
+      <c r="C116">
+        <v>18.27</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>123</v>
+      </c>
+      <c r="C117">
+        <v>15.17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>124</v>
+      </c>
+      <c r="C118">
+        <v>20.61</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated inventory control PVC fittings done
</commit_message>
<xml_diff>
--- a/MakoInventoryControl.xlsx
+++ b/MakoInventoryControl.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>Item:</t>
   </si>
@@ -393,14 +393,161 @@
     <t>4"x3" PVC T</t>
   </si>
   <si>
-    <t>Resume on Page 325 in connors book</t>
+    <t>3"x3"x3"x2" PVC T with Right Inlet</t>
+  </si>
+  <si>
+    <t>3"x3"x3"x2"x2" PVC T with Left &amp; Right Inlet</t>
+  </si>
+  <si>
+    <t>1.5" PVC Double T</t>
+  </si>
+  <si>
+    <t>2" PVC Double T</t>
+  </si>
+  <si>
+    <t>3" PVC Double T</t>
+  </si>
+  <si>
+    <t>4" PVC Double T</t>
+  </si>
+  <si>
+    <t>3"x3"x3"x3"x2"x2" PVC Double T with Left &amp; Right Inlet</t>
+  </si>
+  <si>
+    <r>
+      <t>3"x3"x3"x3"x2" PVC Double T with 90</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>° inlet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>1.5" PVC Y</t>
+  </si>
+  <si>
+    <t>2" PVC Y</t>
+  </si>
+  <si>
+    <t>3" PVC Y</t>
+  </si>
+  <si>
+    <t>4" PVC Y</t>
+  </si>
+  <si>
+    <t>2"x1.5"x1.5" PVC Y</t>
+  </si>
+  <si>
+    <t>2"x1.5"x2" PVC Y</t>
+  </si>
+  <si>
+    <t>2"x2"x1.5" PVC Y</t>
+  </si>
+  <si>
+    <t>3"x3"x1.5" PVC Y</t>
+  </si>
+  <si>
+    <t>3"x3"x2" PVC Y</t>
+  </si>
+  <si>
+    <t>4"x4"x1.5" PVC Y</t>
+  </si>
+  <si>
+    <t>4"x4"x2" PVC Y</t>
+  </si>
+  <si>
+    <t>4"x4"x3" PVC Y</t>
+  </si>
+  <si>
+    <t>1.5" Double Y</t>
+  </si>
+  <si>
+    <t>2" Double Y</t>
+  </si>
+  <si>
+    <t>3" Double Y</t>
+  </si>
+  <si>
+    <t>4" Double Y</t>
+  </si>
+  <si>
+    <t>2"x2"x1.5"x1.5" Double Y</t>
+  </si>
+  <si>
+    <t>3"x3"x1.5"x1.5" Double Y</t>
+  </si>
+  <si>
+    <t>3"x3"x2"x2" Double Y</t>
+  </si>
+  <si>
+    <t>4"x4"x3"x3" Double Y</t>
+  </si>
+  <si>
+    <t>4"x4"x2"x2" Double Y</t>
+  </si>
+  <si>
+    <t>1.5" PVC P-Trap solvent weld</t>
+  </si>
+  <si>
+    <t>2" PVC P-Trap solvent weld</t>
+  </si>
+  <si>
+    <t>3" PVC P-Trap solvent weld</t>
+  </si>
+  <si>
+    <t>4" PVC P-Trap solvent weld</t>
+  </si>
+  <si>
+    <t>1.5" PVC P-Trap w/Plastic Nut</t>
+  </si>
+  <si>
+    <t>2" PVC P-Trap w/Plastic Nut</t>
+  </si>
+  <si>
+    <t>4" PVC Closet Flange Hub End</t>
+  </si>
+  <si>
+    <t>4"x3" PVC Closet Flange Hub End</t>
+  </si>
+  <si>
+    <t>4" PVC Closet Flange w/Knock Out</t>
+  </si>
+  <si>
+    <t>4"x3" PVC Closet Flange w/Knock Out</t>
+  </si>
+  <si>
+    <t>4" Closet Flange w/Adj metal ring - Hub</t>
+  </si>
+  <si>
+    <t>4"x3" Closet Flange w/Adj metal ring - Hub</t>
+  </si>
+  <si>
+    <t>4"x3"  Closet Flange w/Adj metal ring - Offset</t>
+  </si>
+  <si>
+    <t>PVC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +559,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -458,9 +619,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -763,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H119"/>
+  <dimension ref="A1:H161"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,933 +1029,1270 @@
         <v>240</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>0.66</v>
+    <row r="4" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>0.91</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>3.15</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>5.4</v>
+        <v>3.15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>2.0299999999999998</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>5.98</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>4.5999999999999996</v>
+        <v>5.98</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>9.1300000000000008</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>9.6999999999999993</v>
+        <v>9.1300000000000008</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
-        <v>3.68</v>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14">
-        <v>2.57</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15">
-        <v>6.51</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16">
-        <v>12.52</v>
+        <v>6.51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>1.27</v>
+        <v>12.52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>2.16</v>
+        <v>1.27</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>5.79</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20">
-        <v>7.43</v>
+        <v>5.79</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21">
-        <v>1.28</v>
+        <v>7.43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22">
-        <v>1.71</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23">
-        <v>4.74</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24">
-        <v>10.85</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25">
-        <v>2.4</v>
+        <v>10.85</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27">
-        <v>2.85</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
-        <v>2.76</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29">
-        <v>2.5</v>
+        <v>2.76</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30">
-        <v>7.69</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31">
-        <v>2.8</v>
+        <v>7.69</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>3.41</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33">
-        <v>8.2200000000000006</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34">
-        <v>13.09</v>
+        <v>8.2200000000000006</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35">
-        <v>1.6</v>
+        <v>13.09</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36">
-        <v>2.0699999999999998</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37">
-        <v>5.82</v>
+        <v>2.0699999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38">
-        <v>9.57</v>
+        <v>5.82</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39">
-        <v>1.2</v>
+        <v>9.57</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40">
-        <v>1.34</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41">
-        <v>2.39</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42">
-        <v>3.52</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43">
-        <v>2.71</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44">
-        <v>4.51</v>
+        <v>2.71</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45">
-        <v>7.55</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46">
-        <v>10.78</v>
+        <v>7.55</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47">
-        <v>2.65</v>
+        <v>10.78</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48">
-        <v>1.1599999999999999</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49">
-        <v>5.6</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50">
-        <v>2.92</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51">
-        <v>9.74</v>
+        <v>2.92</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52">
-        <v>4.97</v>
+        <v>9.74</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53">
-        <v>8.74</v>
+        <v>4.97</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54">
-        <v>3.52</v>
+        <v>8.74</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55">
-        <v>5.13</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C56">
-        <v>6.59</v>
+        <v>5.13</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C57">
-        <v>11.32</v>
+        <v>6.59</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58">
-        <v>1.42</v>
+        <v>11.32</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59">
-        <v>2.23</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60">
-        <v>6.56</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61">
-        <v>12.91</v>
+        <v>6.56</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62">
-        <v>17.5</v>
+        <v>12.91</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C63">
-        <v>12.94</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64">
-        <v>13.25</v>
+        <v>12.94</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C65">
-        <v>11.41</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C66">
-        <v>22.52</v>
+        <v>11.41</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67">
-        <v>1.83</v>
+        <v>22.52</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C68">
-        <v>2.79</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C69">
-        <v>7.02</v>
+        <v>2.79</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C70">
-        <v>13.21</v>
+        <v>7.02</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C71">
-        <v>3.27</v>
+        <v>13.21</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C72">
-        <v>3.66</v>
+        <v>3.27</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C73">
-        <v>8.35</v>
+        <v>3.66</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C74">
-        <v>15.94</v>
+        <v>8.35</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C75">
-        <v>5.0199999999999996</v>
+        <v>15.94</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C76">
-        <v>5.5</v>
+        <v>5.0199999999999996</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C77">
-        <v>15.14</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C78">
-        <v>23.32</v>
+        <v>15.14</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C79">
-        <v>2.98</v>
+        <v>23.32</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C80">
-        <v>3.83</v>
+        <v>2.98</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C81">
-        <v>12.17</v>
+        <v>3.83</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C82">
-        <v>18.84</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C83">
-        <v>5.97</v>
+        <v>18.84</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C84">
-        <v>7.78</v>
+        <v>5.97</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C85">
-        <v>16.77</v>
+        <v>7.78</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C86">
-        <v>25.2</v>
+        <v>16.77</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C87">
-        <v>1.38</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C88">
-        <v>2</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C89">
-        <v>5.87</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C90">
-        <v>10.29</v>
+        <v>5.87</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C91">
-        <v>1.33</v>
+        <v>10.29</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C92">
-        <v>2.11</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C93">
-        <v>5.56</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C94">
-        <v>9.51</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C95">
-        <v>1.88</v>
+        <v>9.51</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C96">
-        <v>2.33</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C97">
-        <v>5.77</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C98">
-        <v>9.1300000000000008</v>
+        <v>5.77</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C99">
-        <v>5.32</v>
+        <v>9.1300000000000008</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C100">
-        <v>5.69</v>
+        <v>5.32</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C101">
-        <v>8.94</v>
+        <v>5.69</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C102">
-        <v>13.05</v>
+        <v>8.94</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C103">
-        <v>5.56</v>
+        <v>13.05</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C104">
-        <v>7.59</v>
+        <v>5.56</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C105">
-        <v>20.05</v>
+        <v>7.59</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C106">
-        <v>6.99</v>
+        <v>20.05</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C107">
-        <v>10.51</v>
+        <v>6.99</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C108">
-        <v>20.04</v>
+        <v>10.51</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C109">
-        <v>2.4700000000000002</v>
+        <v>20.04</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C110">
-        <v>3.63</v>
+        <v>2.4700000000000002</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C111">
-        <v>9.5399999999999991</v>
+        <v>3.63</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C112">
-        <v>17.53</v>
+        <v>9.5399999999999991</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C113">
-        <v>3.21</v>
+        <v>17.53</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C114">
-        <v>6.97</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C115">
-        <v>7.14</v>
+        <v>6.97</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C116">
-        <v>18.27</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C117">
-        <v>15.17</v>
+        <v>18.27</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C118">
-        <v>20.61</v>
+        <v>15.17</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>124</v>
+      </c>
+      <c r="C119">
+        <v>20.61</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>125</v>
+      </c>
+      <c r="C120">
+        <v>17.37</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>126</v>
+      </c>
+      <c r="C121">
+        <v>26.61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>127</v>
+      </c>
+      <c r="C122">
+        <v>5.48</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>128</v>
+      </c>
+      <c r="C123">
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>129</v>
+      </c>
+      <c r="C124">
+        <v>20.73</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>130</v>
+      </c>
+      <c r="C125">
+        <v>33.35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>131</v>
+      </c>
+      <c r="C126">
+        <v>39.57</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>132</v>
+      </c>
+      <c r="C127">
+        <v>28.2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>133</v>
+      </c>
+      <c r="C128">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>134</v>
+      </c>
+      <c r="C129">
+        <v>4.43</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>135</v>
+      </c>
+      <c r="C130">
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>136</v>
+      </c>
+      <c r="C131">
+        <v>21.68</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>137</v>
+      </c>
+      <c r="C132">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>138</v>
+      </c>
+      <c r="C133">
+        <v>9.57</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>139</v>
+      </c>
+      <c r="C134">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>140</v>
+      </c>
+      <c r="C135">
+        <v>8.08</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>141</v>
+      </c>
+      <c r="C136">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>142</v>
+      </c>
+      <c r="C137">
+        <v>27.01</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>143</v>
+      </c>
+      <c r="C138">
+        <v>13.05</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>144</v>
+      </c>
+      <c r="C139">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>145</v>
+      </c>
+      <c r="C140">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>146</v>
+      </c>
+      <c r="C141">
+        <v>11.28</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>147</v>
+      </c>
+      <c r="C142">
+        <v>23.7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>148</v>
+      </c>
+      <c r="C143">
+        <v>48.08</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>149</v>
+      </c>
+      <c r="C144">
+        <v>10.29</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>150</v>
+      </c>
+      <c r="C145">
+        <v>20.05</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>151</v>
+      </c>
+      <c r="C146">
+        <v>17.670000000000002</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>153</v>
+      </c>
+      <c r="C147">
+        <v>28.83</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>152</v>
+      </c>
+      <c r="C148">
+        <v>38.08</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>154</v>
+      </c>
+      <c r="C149">
+        <v>4.7300000000000004</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>155</v>
+      </c>
+      <c r="C150">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>156</v>
+      </c>
+      <c r="C151">
+        <v>21.66</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>157</v>
+      </c>
+      <c r="C152">
+        <v>49.39</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>158</v>
+      </c>
+      <c r="C153">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>159</v>
+      </c>
+      <c r="C154">
+        <v>13.15</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>160</v>
+      </c>
+      <c r="C155">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>161</v>
+      </c>
+      <c r="C156">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>162</v>
+      </c>
+      <c r="C157">
+        <v>11.46</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>163</v>
+      </c>
+      <c r="C158">
+        <v>6.46</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>164</v>
+      </c>
+      <c r="C159">
+        <v>17.32</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>165</v>
+      </c>
+      <c r="C160">
+        <v>14.82</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>166</v>
+      </c>
+      <c r="C161">
+        <v>19.89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>